<commit_message>
updates to domains on Space service
</commit_message>
<xml_diff>
--- a/rtaa_gis/lpm/utils/RTAA_Domain_Sheets.xlsx
+++ b/rtaa_gis/lpm/utils/RTAA_Domain_Sheets.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\rtaa_gis\rtaa_gis\lpm\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3F65F3AE-A5AE-4D49-887E-E63EFDD8A9B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lease status" sheetId="2" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="141">
   <si>
     <t>Code</t>
   </si>
@@ -393,9 +394,6 @@
     <t>Board Room Service</t>
   </si>
   <si>
-    <t>Non-Assignable</t>
-  </si>
-  <si>
     <t>Hangar</t>
   </si>
   <si>
@@ -417,9 +415,6 @@
     <t>Evidence</t>
   </si>
   <si>
-    <t>Assignable</t>
-  </si>
-  <si>
     <t>Private</t>
   </si>
   <si>
@@ -451,12 +446,15 @@
   </si>
   <si>
     <t>Bridge or Tunnel</t>
+  </si>
+  <si>
+    <t>Leasable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -900,74 +898,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -978,40 +976,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
     </row>
@@ -1022,64 +1015,64 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1090,274 +1083,274 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.88671875" customWidth="1"/>
+    <col min="1" max="1" width="92.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>71</v>
       </c>
@@ -1368,410 +1361,411 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A66"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:A65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1784,12 +1778,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>